<commit_message>
dynamically render npc and locations on maps
</commit_message>
<xml_diff>
--- a/data/locations.xlsx
+++ b/data/locations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marcin\Desktop\Backup\Kolo_game\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{505A2B9C-012D-446C-804A-1D21503B369F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A498191-7FAD-4851-992A-F0AF2DE4B2E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CE50C89C-00FC-4DCB-8E0A-9CB23263FC61}"/>
   </bookViews>
@@ -424,7 +424,7 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
full automation of locations and npc
</commit_message>
<xml_diff>
--- a/data/locations.xlsx
+++ b/data/locations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marcin\Desktop\Backup\Kolo_game\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A498191-7FAD-4851-992A-F0AF2DE4B2E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24CEF7FC-A0C7-468C-9E77-7C6B91E88B69}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CE50C89C-00FC-4DCB-8E0A-9CB23263FC61}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>map</t>
   </si>
@@ -69,6 +69,12 @@
   </si>
   <si>
     <t>TILESIZE</t>
+  </si>
+  <si>
+    <t>next_loc</t>
+  </si>
+  <si>
+    <t>castle</t>
   </si>
 </sst>
 </file>
@@ -421,10 +427,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F260D7A-3AE8-4E1E-B098-59010890A167}">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -440,7 +446,7 @@
     <col min="9" max="9" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -469,10 +475,13 @@
         <v>3</v>
       </c>
       <c r="J1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -486,25 +495,28 @@
         <v>896</v>
       </c>
       <c r="E2">
-        <f>C2+150-J2</f>
+        <f>C2+150-K2</f>
         <v>1110</v>
       </c>
       <c r="F2">
-        <f>C2+150+0.5*J2</f>
+        <f>C2+150+0.5*K2</f>
         <v>1206</v>
       </c>
       <c r="G2">
-        <f>D2+300-J2</f>
+        <f>D2+300-K2</f>
         <v>1132</v>
       </c>
       <c r="H2">
-        <f>D2+300-0.25*J2</f>
+        <f>D2+300-0.25*K2</f>
         <v>1180</v>
       </c>
       <c r="I2" t="s">
         <v>10</v>
       </c>
-      <c r="J2">
+      <c r="J2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2">
         <v>64</v>
       </c>
     </row>

</xml_diff>

<commit_message>
locations - tree graph
</commit_message>
<xml_diff>
--- a/data/locations.xlsx
+++ b/data/locations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marcin\Desktop\Backup\Kolo_game\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24CEF7FC-A0C7-468C-9E77-7C6B91E88B69}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E4A9E66-AE25-48BF-BD22-71B34EA6BE61}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CE50C89C-00FC-4DCB-8E0A-9CB23263FC61}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
   <si>
     <t>map</t>
   </si>
@@ -75,6 +75,9 @@
   </si>
   <si>
     <t>castle</t>
+  </si>
+  <si>
+    <t>first_map</t>
   </si>
 </sst>
 </file>
@@ -427,10 +430,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F260D7A-3AE8-4E1E-B098-59010890A167}">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -495,19 +498,19 @@
         <v>896</v>
       </c>
       <c r="E2">
-        <f>C2+150-K2</f>
+        <f>C2+150-K$2</f>
         <v>1110</v>
       </c>
       <c r="F2">
-        <f>C2+150+0.5*K2</f>
+        <f>C2+150+0.5*K$2</f>
         <v>1206</v>
       </c>
       <c r="G2">
-        <f>D2+300-K2</f>
+        <f>D2+300-K$2</f>
         <v>1132</v>
       </c>
       <c r="H2">
-        <f>D2+300-0.25*K2</f>
+        <f>D2+300-0.25*K$2</f>
         <v>1180</v>
       </c>
       <c r="I2" t="s">
@@ -518,6 +521,42 @@
       </c>
       <c r="K2">
         <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3">
+        <v>1024</v>
+      </c>
+      <c r="D3">
+        <v>896</v>
+      </c>
+      <c r="E3">
+        <f>C3+150-K$2</f>
+        <v>1110</v>
+      </c>
+      <c r="F3">
+        <f>C3+150+0.5*K$2</f>
+        <v>1206</v>
+      </c>
+      <c r="G3">
+        <f>D3+300-K$2</f>
+        <v>1132</v>
+      </c>
+      <c r="H3">
+        <f>D3+300-0.25*K$2</f>
+        <v>1180</v>
+      </c>
+      <c r="I3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J3" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>